<commit_message>
SQL edits and Dashboard Personal updates
</commit_message>
<xml_diff>
--- a/Other/Notes/UserAttributes.xlsx
+++ b/Other/Notes/UserAttributes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="26">
   <si>
     <t>UserModel</t>
   </si>
@@ -441,16 +441,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -500,6 +502,9 @@
       <c r="E3" t="s">
         <v>18</v>
       </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -777,10 +782,15 @@
       <c r="B20" t="s">
         <v>2</v>
       </c>
-      <c r="C20" t="s">
+      <c r="F20" t="s">
         <v>25</v>
       </c>
-      <c r="F20" t="s">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>